<commit_message>
Completed up to checkpoint 3.
</commit_message>
<xml_diff>
--- a/InvestmentAssignment/Investments.xlsx
+++ b/InvestmentAssignment/Investments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t xml:space="preserve">Table-1.1</t>
   </si>
@@ -332,10 +332,19 @@
     <t xml:space="preserve">Top English speaking country</t>
   </si>
   <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Second English speaking country</t>
   </si>
   <si>
+    <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Third English speaking country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN</t>
   </si>
   <si>
     <t xml:space="preserve">Table - 5.1</t>
@@ -580,7 +589,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -647,10 +656,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -921,7 +926,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -969,7 +974,7 @@
       <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="n">
+      <c r="C5" s="15" t="n">
         <v>11749430.94</v>
       </c>
     </row>
@@ -980,7 +985,7 @@
       <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="17" t="n">
+      <c r="C6" s="15" t="n">
         <v>958694.47</v>
       </c>
     </row>
@@ -991,7 +996,7 @@
       <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="17" t="n">
+      <c r="C7" s="15" t="n">
         <v>719719.06</v>
       </c>
     </row>
@@ -1002,7 +1007,7 @@
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="17" t="n">
+      <c r="C8" s="15" t="n">
         <v>73341461.74</v>
       </c>
     </row>
@@ -1010,13 +1015,13 @@
       <c r="A9" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1058,8 +1063,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1071,14 +1076,14 @@
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
@@ -1088,42 +1093,48 @@
       <c r="C3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+      <c r="A5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
+      <c r="A6" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
+      <c r="B6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="22"/>
+      <c r="B7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1163,7 +1174,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.85"/>
@@ -1171,147 +1182,147 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.85"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" s="24" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+    <row r="1" s="23" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" s="23" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>32</v>
+      <c r="C4" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="n">
+      <c r="A5" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>33</v>
+      <c r="B5" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="n">
+      <c r="A6" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>34</v>
+      <c r="B6" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="n">
+      <c r="A7" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>35</v>
+      <c r="B7" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="n">
+      <c r="A8" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>36</v>
+      <c r="B8" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="n">
+      <c r="A9" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>37</v>
+      <c r="B9" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="n">
+      <c r="A10" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>38</v>
+      <c r="B10" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="n">
+      <c r="A11" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>39</v>
+      <c r="B11" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="n">
+      <c r="A12" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>40</v>
+      <c r="B12" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="n">
+      <c r="A13" s="29" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>41</v>
+      <c r="B13" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="n">
+      <c r="A14" s="29" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>42</v>
+      <c r="B14" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>

</xml_diff>

<commit_message>
Completed upto checkpoint 5. The notebook also contains the output to every cell.
</commit_message>
<xml_diff>
--- a/InvestmentAssignment/Investments.xlsx
+++ b/InvestmentAssignment/Investments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t xml:space="preserve">Table-1.1</t>
   </si>
@@ -356,15 +356,6 @@
     <t xml:space="preserve">Sl.no</t>
   </si>
   <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total number of Investments (count)</t>
   </si>
   <si>
@@ -374,12 +365,21 @@
     <t xml:space="preserve">Top Sector name (no. of investment-wise)</t>
   </si>
   <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleantech / Semiconductors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Second Sector name (no. of investment-wise)</t>
   </si>
   <si>
     <t xml:space="preserve">Third Sector name (no. of investment-wise)</t>
   </si>
   <si>
+    <t xml:space="preserve">Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of investments in top sector (3)</t>
   </si>
   <si>
@@ -392,7 +392,25 @@
     <t xml:space="preserve">For point 3 (top sector count-wise), which company received the highest investment?</t>
   </si>
   <si>
+    <t xml:space="preserve">SoFi (/organization/social-finance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OneWeb (/organization/oneweb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram Power (/organization/ram-power)</t>
+  </si>
+  <si>
     <t xml:space="preserve">For point 4 (second best sector count-wise), which company received the highest investment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freescale Semiconductor (/organization/freescale)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunocore (/organization/immunocore)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D2L (/organization/desire2learn)</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1081,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1166,19 +1184,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.85"/>
   </cols>
   <sheetData>
@@ -1209,125 +1227,188 @@
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>35421</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>2120</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>1256</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>414502753027.06</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>21321274230.84</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>9655574999.23</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="9" t="n">
+        <v>8693</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>571</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="9" t="n">
+        <v>8113</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>456</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="n">
         <v>8</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="9" t="n">
+        <v>5553</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>359</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="n">
         <v>9</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="n">
         <v>10</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
+        <v>48</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B2"/>
@@ -1353,7 +1434,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E14">
+  <conditionalFormatting sqref="A5:E6 A10:E13 A7:C9 A14:D14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1375,6 +1456,66 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>